<commit_message>
add case study tests
</commit_message>
<xml_diff>
--- a/Chapter_3_Data_Analysis_in_Pandas/files/test_out.xlsx
+++ b/Chapter_3_Data_Analysis_in_Pandas/files/test_out.xlsx
@@ -16,13 +16,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
+    <t>a</t>
+  </si>
+  <si>
     <t>b</t>
   </si>
   <si>
     <t>c</t>
-  </si>
-  <si>
-    <t>d</t>
   </si>
 </sst>
 </file>
@@ -380,7 +380,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -399,21 +399,43 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
         <v>4</v>
-      </c>
-      <c r="B2">
-        <v>6</v>
-      </c>
-      <c r="C2">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2</v>
+      </c>
       <c r="B3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C3">
-        <v>6</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>